<commit_message>
fixed comp pin mapping on variants fixed scripts
</commit_message>
<xml_diff>
--- a/Lattice/iCE40-LP4K-CM81.xlsx
+++ b/Lattice/iCE40-LP4K-CM81.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="162">
   <si>
     <t xml:space="preserve">PIN</t>
   </si>
@@ -181,10 +181,16 @@
     <t xml:space="preserve">GNDPLL0</t>
   </si>
   <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
     <t xml:space="preserve">J6</t>
   </si>
   <si>
     <t xml:space="preserve">VCCPLL0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U</t>
   </si>
   <si>
     <t xml:space="preserve">J7</t>
@@ -514,6 +520,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -597,14 +604,14 @@
   </sheetPr>
   <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="2.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="3.79"/>
   </cols>
@@ -966,8 +973,11 @@
       <c r="B26" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="C26" s="0" t="s">
+        <v>53</v>
+      </c>
       <c r="D26" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -975,10 +985,13 @@
         <v>0</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>56</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -986,13 +999,13 @@
         <v>0</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1000,13 +1013,13 @@
         <v>0</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1014,13 +1027,13 @@
         <v>0</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1028,13 +1041,13 @@
         <v>0</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1042,13 +1055,13 @@
         <v>0</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1056,13 +1069,13 @@
         <v>0</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1070,13 +1083,13 @@
         <v>0</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1084,13 +1097,13 @@
         <v>0</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1098,13 +1111,13 @@
         <v>0</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1112,13 +1125,13 @@
         <v>0</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1126,13 +1139,13 @@
         <v>0</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1140,13 +1153,13 @@
         <v>0</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1154,13 +1167,13 @@
         <v>0</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1168,13 +1181,13 @@
         <v>0</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1182,13 +1195,13 @@
         <v>0</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1196,13 +1209,13 @@
         <v>0</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1210,13 +1223,13 @@
         <v>0</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1224,13 +1237,13 @@
         <v>0</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C45" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1238,13 +1251,13 @@
         <v>0</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C46" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1252,13 +1265,13 @@
         <v>0</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C47" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1266,13 +1279,13 @@
         <v>0</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C48" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1280,13 +1293,13 @@
         <v>0</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C49" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1294,13 +1307,13 @@
         <v>0</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C50" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1308,13 +1321,13 @@
         <v>0</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C51" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1322,13 +1335,13 @@
         <v>0</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C52" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1336,13 +1349,13 @@
         <v>0</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C53" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1350,13 +1363,13 @@
         <v>0</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C54" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1364,13 +1377,13 @@
         <v>0</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C55" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1378,13 +1391,13 @@
         <v>0</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C56" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1392,13 +1405,13 @@
         <v>0</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C57" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1406,13 +1419,13 @@
         <v>0</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C58" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1420,13 +1433,13 @@
         <v>0</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C59" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1434,13 +1447,13 @@
         <v>0</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C60" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1448,13 +1461,13 @@
         <v>0</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C61" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1462,13 +1475,13 @@
         <v>0</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C62" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1476,13 +1489,13 @@
         <v>0</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C63" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1490,13 +1503,13 @@
         <v>0</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C64" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1504,13 +1517,13 @@
         <v>0</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1518,13 +1531,13 @@
         <v>0</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1532,13 +1545,13 @@
         <v>0</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1546,13 +1559,13 @@
         <v>0</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C68" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1560,13 +1573,13 @@
         <v>0</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1574,13 +1587,13 @@
         <v>0</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1588,13 +1601,13 @@
         <v>0</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1602,13 +1615,13 @@
         <v>0</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1616,13 +1629,13 @@
         <v>0</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1630,13 +1643,13 @@
         <v>0</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1644,13 +1657,13 @@
         <v>0</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1658,13 +1671,13 @@
         <v>0</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1672,13 +1685,13 @@
         <v>0</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1686,13 +1699,13 @@
         <v>0</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1700,13 +1713,13 @@
         <v>0</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1714,13 +1727,13 @@
         <v>0</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1728,13 +1741,13 @@
         <v>0</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>